<commit_message>
Split the reports details in two different lists (second part)
</commit_message>
<xml_diff>
--- a/hp-sla-analyser/src/main/resources/files/reportTemplate.xlsx
+++ b/hp-sla-analyser/src/main/resources/files/reportTemplate.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
   </bookViews>
   <sheets>
-    <sheet name="Report C - Salida" sheetId="4" r:id="rId1"/>
+    <sheet name="flagged IM's" sheetId="4" r:id="rId1"/>
+    <sheet name="undetermined" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="3873892070"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Incident Identifier</t>
   </si>
@@ -606,6 +607,1150 @@
   <dimension ref="A1:Z24760"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="4" customWidth="1"/>
+    <col min="11" max="12" width="13.42578125" style="4" customWidth="1"/>
+    <col min="13" max="14" width="6.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.5703125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.28515625" style="4" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23739" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23740" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23741" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23742" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23743" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23744" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23745" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23746" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23747" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23748" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23749" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23750" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23751" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23752" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23753" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23754" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23755" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23756" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23757" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23758" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23759" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23760" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23761" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23762" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23763" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23764" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23765" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23766" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23767" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23768" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23769" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23770" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23771" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23772" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23773" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23774" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23775" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23776" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23777" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23778" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23779" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23780" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23781" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23782" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23783" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23784" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23785" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23786" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23787" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23788" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23789" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23790" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23791" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23792" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23793" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23794" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23795" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23796" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23797" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23798" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23799" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23800" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23801" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23802" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23803" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23804" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23805" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23806" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23807" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23808" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23809" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23810" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23811" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23812" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23813" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23814" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23815" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23816" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23817" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23818" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23819" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23820" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23821" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23822" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23823" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23824" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23825" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23826" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23827" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23828" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23829" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23830" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23831" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23832" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23833" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23834" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23835" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23836" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23837" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23838" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23839" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23840" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23841" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23842" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23843" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23844" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23845" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23846" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23847" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23848" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23849" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23850" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23851" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23852" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23853" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23854" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23855" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23856" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23857" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23858" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23859" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23860" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23861" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23862" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23863" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23864" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23865" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23866" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23867" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23868" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23869" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23870" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23871" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23872" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23873" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23874" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23875" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23876" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23877" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23878" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23879" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23880" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23881" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23882" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23883" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23884" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23885" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23886" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23887" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23888" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23889" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23890" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23891" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23892" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23893" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23894" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23895" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23896" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23897" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23898" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23899" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23900" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23901" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23902" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23903" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23904" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23905" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23906" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23907" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23908" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23909" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23910" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23911" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23912" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23913" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23914" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23915" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23916" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23917" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23918" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23919" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23920" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23921" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23922" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23923" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23924" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23925" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23926" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23927" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23928" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23929" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23930" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23931" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23932" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23933" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23934" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23935" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23936" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23937" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23938" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23939" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23940" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23941" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23942" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23943" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23944" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23945" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23946" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23947" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23948" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23949" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23950" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23951" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23952" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23953" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23954" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23955" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23956" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23957" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23958" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23959" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23960" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23961" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23962" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23963" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23964" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23965" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23966" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23967" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23968" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23969" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23970" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23971" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23972" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23973" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23974" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23975" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23976" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23977" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23978" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23979" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23980" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23981" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23982" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23983" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23984" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23985" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23986" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23987" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23988" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23989" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23990" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23991" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23992" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23993" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23994" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23995" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23996" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23997" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23998" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23999" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24000" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24001" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24002" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24003" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24004" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24005" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24006" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24007" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24008" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24009" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24010" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24011" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24012" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24013" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24014" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24015" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24016" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24017" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24018" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24019" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24020" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24021" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24022" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24023" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24024" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24025" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24026" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24027" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24028" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24029" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24030" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24031" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24032" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24033" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24034" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24035" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24036" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24037" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24038" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24039" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24040" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24041" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24042" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24043" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24044" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24045" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24046" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24047" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24048" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24049" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24050" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24051" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24052" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24053" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24054" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24055" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24056" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24057" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24058" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24059" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24060" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24061" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24062" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24063" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24064" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24065" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24066" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24067" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24068" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24069" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24070" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24071" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24072" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24073" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24074" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24075" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24076" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24077" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24078" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24079" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24080" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24081" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24082" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24083" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24084" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24085" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24086" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24087" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24088" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24089" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24090" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24091" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24092" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24093" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24094" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24095" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24096" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24097" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24098" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24099" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24100" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24101" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24102" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24103" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24104" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24105" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24106" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24107" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24108" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24109" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24110" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24111" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24112" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24113" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24114" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24115" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24116" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24117" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24118" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24119" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24120" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24121" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24122" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24123" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24124" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24125" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24126" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24127" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24128" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24129" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24130" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24131" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24132" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24133" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24134" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24135" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24136" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24137" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24138" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24139" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24140" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24141" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24142" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24143" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24144" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24145" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24146" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24147" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24148" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24149" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24150" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24151" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24152" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24153" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24154" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24155" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24156" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24157" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24158" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24159" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24160" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24161" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24162" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24163" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24164" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24165" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24166" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24167" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24168" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24169" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24170" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24171" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24172" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24173" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24174" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24175" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24176" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24177" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24178" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24179" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24180" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24181" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24182" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24183" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24184" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24185" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24186" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24187" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24188" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24189" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24190" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24191" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24192" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24193" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24194" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24195" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24196" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24197" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24198" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24199" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24200" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24201" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24202" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24203" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24204" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24205" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24206" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24207" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24208" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24209" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24210" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24211" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24212" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24213" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24214" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24215" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24216" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24217" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24218" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24219" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24220" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24221" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24222" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24223" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24224" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24225" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24226" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24227" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24228" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24229" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24230" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24231" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24232" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24233" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24234" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24235" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24236" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24237" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24238" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24239" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24240" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24241" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24242" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24243" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24244" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24245" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24246" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24247" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24248" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24249" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24250" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24251" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24252" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24253" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24254" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24255" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24256" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24257" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24258" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24259" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24260" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24261" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24262" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24263" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24264" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24265" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24266" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24267" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24268" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24269" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24270" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24271" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24272" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24273" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24274" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24275" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24276" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24277" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24278" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24279" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24280" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24281" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24282" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24283" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24284" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24285" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24286" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24287" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24288" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24289" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24290" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24291" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24292" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24293" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24294" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24295" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24296" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24297" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24298" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24299" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24300" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24301" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24302" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24303" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24304" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24305" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24306" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24307" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24308" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24309" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24310" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24311" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24312" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24313" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24314" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24315" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24316" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24317" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24318" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24319" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24320" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24321" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24322" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24323" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24324" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24325" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24326" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24327" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24328" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24329" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24330" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24331" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24332" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24333" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24334" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24335" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24336" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24337" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24338" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24339" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24340" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24341" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24342" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24343" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24344" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24345" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24346" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24347" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24348" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24349" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24350" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24351" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24352" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24353" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24354" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24355" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24356" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24357" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24358" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24359" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24360" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24361" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24362" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24363" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24364" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24365" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24366" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24367" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24368" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24369" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24370" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24371" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24372" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24373" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24374" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24375" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24376" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24377" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24378" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24379" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24380" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24381" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24382" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24383" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24384" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24385" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24386" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24387" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24388" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24389" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24390" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24391" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24392" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24393" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24394" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24395" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24396" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24397" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24398" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24399" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24400" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24401" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24402" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24403" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24404" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24405" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24406" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24407" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24408" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24409" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24410" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24411" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24412" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24413" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24414" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24415" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24416" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24417" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24418" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24419" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24420" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24421" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24422" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24423" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24424" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24425" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24426" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24427" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24428" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24429" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24430" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24431" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24432" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24433" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24434" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24435" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24436" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24437" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24438" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24439" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24440" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24441" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24442" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24443" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24444" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24445" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24446" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24447" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24448" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24449" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24450" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24451" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24452" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24453" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24454" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24455" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24456" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24457" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24458" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24459" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24460" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24461" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24462" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24463" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24464" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24465" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24466" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24467" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24468" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24469" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24470" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24471" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24472" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24473" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24474" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24475" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24476" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24477" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24478" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24479" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24480" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24481" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24482" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24483" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24484" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24485" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24486" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24487" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24488" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24489" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24490" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24491" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24492" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24493" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24494" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24495" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24496" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24497" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24498" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24499" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24500" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24501" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24502" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24503" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24504" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24505" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24506" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24507" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24508" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24509" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24510" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24511" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24512" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24513" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24514" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24515" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24516" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24517" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24518" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24519" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24520" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24521" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24522" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24523" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24524" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24525" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24526" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24527" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24528" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24529" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24530" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24531" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24532" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24533" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24534" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24535" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24536" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24537" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24538" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24539" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24540" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24541" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24542" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24543" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24544" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24545" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24546" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24547" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24548" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24549" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24550" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24551" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24552" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24553" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24554" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24555" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24556" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24557" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24558" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24559" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24560" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24561" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24562" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24563" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24564" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24565" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24566" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24567" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24568" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24569" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24570" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24571" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24572" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24573" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24574" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24575" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24576" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24577" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24578" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24579" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24580" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24581" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24582" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24583" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24584" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24585" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24586" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24587" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24588" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24589" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24590" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24591" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24592" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24593" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24594" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24595" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24596" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24597" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24598" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24599" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24600" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24601" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24602" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24603" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24604" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24605" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24606" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24607" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24608" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24609" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24610" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24611" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24612" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24613" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24614" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24615" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24616" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24617" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24618" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24619" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24620" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24621" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24622" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24623" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24624" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24625" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24626" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24627" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24628" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24629" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24630" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24631" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24632" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24633" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24634" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24635" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24636" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24637" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24638" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24639" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24640" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24641" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24642" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24643" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24644" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24645" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24646" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24647" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24648" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24649" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24650" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24651" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24652" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24653" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24654" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24655" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24656" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24657" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24658" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24659" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24660" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24661" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24662" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24663" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24664" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24665" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24666" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24667" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24668" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24669" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24670" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24671" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24672" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24673" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24674" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24675" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24676" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24677" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24678" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24679" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24680" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24681" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24682" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24683" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24684" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24685" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24686" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24687" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24688" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24689" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24690" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24691" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24692" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24693" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24694" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24695" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24696" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24697" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24698" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24699" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24700" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24701" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24702" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24703" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24704" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24705" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24706" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24707" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24708" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24709" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24710" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24711" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24712" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24713" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24714" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24715" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24716" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24717" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24718" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24719" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24720" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24721" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24722" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24723" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24724" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24725" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24726" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24727" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24728" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24729" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24730" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24731" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24732" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24733" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24734" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24735" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24736" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24737" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24738" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24739" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24740" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24741" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24742" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24743" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24744" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24745" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24746" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24747" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24748" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24749" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24750" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24751" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24752" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24753" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24754" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24755" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24756" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24757" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24758" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24759" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24760" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z24760"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix cell styles accordingly to the template
</commit_message>
<xml_diff>
--- a/hp-sla-analyser/src/main/resources/files/reportTemplate.xlsx
+++ b/hp-sla-analyser/src/main/resources/files/reportTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Incident Identifier</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Error Details</t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <dimension ref="A1:Z24760"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -716,6 +719,11 @@
       </c>
       <c r="Z1" s="2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23739" s="6" customFormat="1" x14ac:dyDescent="0.2"/>

</xml_diff>